<commit_message>
Modifier le pdf Questionnaire ..Kimma Bghat Hafsa Justify  ;)
</commit_message>
<xml_diff>
--- a/Êtude Financière/Etude.F TakeTaxi.xlsx
+++ b/Êtude Financière/Etude.F TakeTaxi.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ayoub\Desktop\TakeTaxi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\taketaxi_template\Êtude Financière\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{401579F2-D05F-42F0-A2A0-A8C0E00B644B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bilan 1ere Année" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
     <sheet name="Bilan Final" sheetId="3" r:id="rId7"/>
     <sheet name="Calcule" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="105">
   <si>
     <t>Active</t>
   </si>
@@ -334,12 +335,24 @@
   </si>
   <si>
     <t xml:space="preserve">              Frais de création</t>
+  </si>
+  <si>
+    <t>Ratio d’indépendance financière = Capitaux propres / Capitaux permanents</t>
+  </si>
+  <si>
+    <t>Ratio de liquidité générale = Actif circulant / Passif circulant</t>
+  </si>
+  <si>
+    <t>Délai de paiement des clients = (Créances clients * 360) / ventes TTC</t>
+  </si>
+  <si>
+    <t>Délai de paiement des fournisseurs = (Dettes fournisseurs * 360) / achats TTC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -506,7 +519,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -535,10 +548,16 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
@@ -547,17 +566,17 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -565,42 +584,42 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="3" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="3" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="4" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="2" builtinId="18"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Titre 1" xfId="1" builtinId="16"/>
-    <cellStyle name="Titre 2" xfId="4" builtinId="17"/>
-    <cellStyle name="Titre 3" xfId="2" builtinId="18"/>
     <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
   <dxfs count="4">
@@ -651,7 +670,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -696,7 +721,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
+        <xdr:cNvPr id="5" name="Connecteur droit 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -746,7 +777,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -795,7 +832,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
+        <xdr:cNvPr id="7" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -844,7 +887,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="9" name="Connecteur droit 8"/>
+        <xdr:cNvPr id="9" name="Connecteur droit 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -898,7 +947,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="2" name="Connecteur droit 1"/>
+        <xdr:cNvPr id="2" name="Connecteur droit 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -947,7 +1002,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -996,7 +1057,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connecteur droit 3"/>
+        <xdr:cNvPr id="4" name="Connecteur droit 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1050,7 +1117,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="8" name="Connecteur droit 7"/>
+        <xdr:cNvPr id="8" name="Connecteur droit 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000008000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1099,7 +1172,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="15" name="Connecteur droit 14"/>
+        <xdr:cNvPr id="15" name="Connecteur droit 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-00000F000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1148,7 +1227,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="16" name="Connecteur droit 15"/>
+        <xdr:cNvPr id="16" name="Connecteur droit 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000010000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1202,7 +1287,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="3" name="Connecteur droit 2"/>
+        <xdr:cNvPr id="3" name="Connecteur droit 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1247,7 +1338,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="4" name="Connecteur droit 3"/>
+        <xdr:cNvPr id="4" name="Connecteur droit 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1292,7 +1389,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="5" name="Connecteur droit 4"/>
+        <xdr:cNvPr id="5" name="Connecteur droit 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1337,7 +1440,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="6" name="Connecteur droit 5"/>
+        <xdr:cNvPr id="6" name="Connecteur droit 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1382,7 +1491,13 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="7" name="Connecteur droit 6"/>
+        <xdr:cNvPr id="7" name="Connecteur droit 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0600-000007000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -1416,75 +1531,75 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Tableau37" displayName="Tableau37" ref="M2:N11" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tableau37" displayName="Tableau37" ref="M2:N11" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Colonne2" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Tableau378" displayName="Tableau378" ref="H7:I20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tableau378" displayName="Tableau378" ref="H7:I20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Colonne2" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Tableau379" displayName="Tableau379" ref="M2:N12" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Tableau379" displayName="Tableau379" ref="M2:N12" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="2">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataDxfId="3" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="Colonne2" dataDxfId="3" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Tableau37810" displayName="Tableau37810" ref="H7:J20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tableau37810" displayName="Tableau37810" ref="H7:J20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Colonne2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Tableau37810512" displayName="Tableau37810512" ref="L3:N17" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Tableau37810512" displayName="Tableau37810512" ref="L3:N17" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="Colonne2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Tableau378105" displayName="Tableau378105" ref="H7:J20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Tableau378105" displayName="Tableau378105" ref="H7:J20" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="3">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Colonne2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Colonne3" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Tableau3786" displayName="Tableau3786" ref="A1:D14" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Tableau3786" displayName="Tableau3786" ref="A1:D14" headerRowCount="0" totalsRowShown="0" headerRowCellStyle="Normal" dataCellStyle="Normal">
   <tableColumns count="4">
-    <tableColumn id="1" name="Colonne1" dataCellStyle="Normal"/>
-    <tableColumn id="2" name="Colonne2" dataDxfId="2" dataCellStyle="Normal"/>
-    <tableColumn id="3" name="Colonne3" dataDxfId="1" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
-    <tableColumn id="4" name="Colonne4" dataDxfId="0" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Colonne1" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Colonne2" dataDxfId="2" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Colonne3" dataDxfId="1" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Colonne4" dataDxfId="0" headerRowCellStyle="Normal" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -1752,14 +1867,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="124" workbookViewId="0">
-      <selection sqref="A1:J14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" zoomScaleSheetLayoutView="124" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24:H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="11.42578125" customWidth="1"/>
@@ -1775,38 +1890,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="39" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="19"/>
       <c r="M2" t="s">
         <v>62</v>
       </c>
@@ -1815,26 +1930,26 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14">
         <f>D4+D6+D5</f>
         <v>69500</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14">
         <f>I4+I5</f>
         <v>90000</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="15"/>
       <c r="M3" t="s">
         <v>68</v>
       </c>
@@ -1843,25 +1958,25 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14">
         <f>N3*N11</f>
         <v>50000</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14">
         <v>80000</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="M4" t="s">
         <v>69</v>
       </c>
@@ -1870,24 +1985,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14">
         <v>2000</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14">
         <v>10000</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="M5" t="s">
         <v>70</v>
       </c>
@@ -1896,20 +2011,20 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14">
         <v>17500</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="M6" t="s">
         <v>71</v>
       </c>
@@ -1918,26 +2033,26 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14">
         <f>D8</f>
         <v>35000</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
         <f>I8+I9+I10</f>
         <v>31000</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="15"/>
       <c r="L7" s="8"/>
       <c r="M7" t="s">
         <v>63</v>
@@ -1947,25 +2062,25 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14">
         <f>N3*N5+N4*N6</f>
         <v>35000</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>5000</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="M8" t="s">
         <v>67</v>
       </c>
@@ -1974,20 +2089,20 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14">
         <v>1000</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="14"/>
       <c r="M9" t="s">
         <v>72</v>
       </c>
@@ -1996,20 +2111,20 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14">
         <v>25000</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="14"/>
       <c r="M10" t="s">
         <v>73</v>
       </c>
@@ -2018,23 +2133,23 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14">
         <f>SUM(D12:E13)</f>
         <v>16500</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
       <c r="M11" t="s">
         <v>77</v>
       </c>
@@ -2043,78 +2158,230 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17">
         <v>5000</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
         <v>11500</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17">
         <f>D11+D7+D3</f>
         <v>121000</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="18">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17">
         <f>I3+I7</f>
         <v>121000</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="17"/>
     </row>
     <row r="15" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:10" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="34"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="34"/>
+      <c r="I20" s="34"/>
+      <c r="J20" s="34"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="35"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="35"/>
+      <c r="F21" s="35"/>
+      <c r="G21" s="35"/>
+      <c r="H21" s="35"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="35"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="35"/>
+      <c r="E22" s="35"/>
+      <c r="F22" s="35"/>
+      <c r="G22" s="35"/>
+      <c r="H22" s="35"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="35"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="35"/>
+      <c r="H23" s="35"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="35"/>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="35"/>
+      <c r="F24" s="35"/>
+      <c r="G24" s="35"/>
+      <c r="H24" s="35"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="35"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="35"/>
+      <c r="D25" s="35"/>
+      <c r="E25" s="35"/>
+      <c r="F25" s="35"/>
+      <c r="G25" s="35"/>
+      <c r="H25" s="35"/>
+      <c r="I25" s="35"/>
+      <c r="J25" s="35"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" s="35"/>
+      <c r="B26" s="35"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="35"/>
+      <c r="G26" s="35"/>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="35"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" s="35"/>
+      <c r="B27" s="35"/>
+      <c r="C27" s="35"/>
+      <c r="D27" s="35"/>
+      <c r="E27" s="35"/>
+      <c r="F27" s="35"/>
+      <c r="G27" s="35"/>
+      <c r="H27" s="35"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" s="35"/>
+      <c r="B28" s="35"/>
+      <c r="C28" s="35"/>
+      <c r="D28" s="35"/>
+      <c r="E28" s="35"/>
+      <c r="F28" s="35"/>
+      <c r="G28" s="35"/>
+      <c r="H28" s="35"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" s="35"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
+      <c r="D29" s="35"/>
+      <c r="E29" s="35"/>
+      <c r="F29" s="35"/>
+      <c r="G29" s="35"/>
+      <c r="H29" s="35"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
+    </row>
   </sheetData>
-  <mergeCells count="53">
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
+  <mergeCells count="72">
+    <mergeCell ref="A29:H29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="A26:H26"/>
+    <mergeCell ref="I26:J26"/>
+    <mergeCell ref="A27:H27"/>
+    <mergeCell ref="I27:J27"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="A23:H23"/>
+    <mergeCell ref="I23:J23"/>
+    <mergeCell ref="A24:H24"/>
+    <mergeCell ref="I24:J24"/>
+    <mergeCell ref="A25:H25"/>
+    <mergeCell ref="I25:J25"/>
+    <mergeCell ref="A20:J20"/>
+    <mergeCell ref="A21:H21"/>
+    <mergeCell ref="I21:J21"/>
+    <mergeCell ref="A22:H22"/>
+    <mergeCell ref="I22:J22"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
     <mergeCell ref="F14:H14"/>
     <mergeCell ref="A10:C10"/>
     <mergeCell ref="D10:E10"/>
@@ -2131,27 +2398,24 @@
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F6:H6"/>
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:J14">
     <cfRule type="colorScale" priority="5">
@@ -2183,14 +2447,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11:F11"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.5703125" style="7" customWidth="1"/>
     <col min="7" max="7" width="39" customWidth="1"/>
@@ -2199,70 +2463,70 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="25">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="26">
         <f>SUM(E5,E4)</f>
         <v>783250</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="22">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="24">
         <f>I8*I10+I9*I11</f>
         <v>35000</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="25"/>
       <c r="G4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="22">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24">
         <f>(I8*I12*I14+I8*I13*I15)*365</f>
         <v>748250</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" t="s">
         <v>75</v>
       </c>
@@ -2271,29 +2535,29 @@
       <c r="A6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="27">
         <f>SUM(E7:F12)</f>
         <v>788500</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="27">
         <f>1000*50+17500</f>
         <v>67500</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="28"/>
       <c r="H7" t="s">
         <v>62</v>
       </c>
@@ -2303,16 +2567,16 @@
     </row>
     <row r="8" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="27">
         <f>4000*12</f>
         <v>48000</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
       <c r="H8" t="s">
         <v>68</v>
       </c>
@@ -2322,15 +2586,15 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="27">
         <v>12000</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="27"/>
       <c r="H9" t="s">
         <v>69</v>
       </c>
@@ -2340,15 +2604,15 @@
     </row>
     <row r="10" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="22">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="24">
         <v>6000</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="25"/>
       <c r="H10" t="s">
         <v>70</v>
       </c>
@@ -2358,15 +2622,15 @@
     </row>
     <row r="11" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26">
         <v>648000</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="23"/>
       <c r="H11" t="s">
         <v>71</v>
       </c>
@@ -2376,15 +2640,15 @@
     </row>
     <row r="12" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26">
         <v>7000</v>
       </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="23"/>
       <c r="H12" t="s">
         <v>63</v>
       </c>
@@ -2396,16 +2660,16 @@
       <c r="A13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="21">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="27">
         <f>E3-E6</f>
         <v>-5250</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="28"/>
       <c r="H13" t="s">
         <v>67</v>
       </c>
@@ -2417,16 +2681,16 @@
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="21">
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="27">
         <f>E15</f>
         <v>10000</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="28"/>
       <c r="H14" t="s">
         <v>72</v>
       </c>
@@ -2436,15 +2700,15 @@
     </row>
     <row r="15" spans="1:9" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="24">
         <v>10000</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="25"/>
       <c r="H15" t="s">
         <v>73</v>
       </c>
@@ -2456,16 +2720,16 @@
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="27">
         <f>E17</f>
         <v>500</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="28"/>
       <c r="H16" t="s">
         <v>79</v>
       </c>
@@ -2475,15 +2739,15 @@
     </row>
     <row r="17" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="27">
         <v>500</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="28"/>
       <c r="H17" t="s">
         <v>80</v>
       </c>
@@ -2495,16 +2759,16 @@
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="21">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="27">
         <f>E14-E16</f>
         <v>9500</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="28"/>
       <c r="H18" t="s">
         <v>81</v>
       </c>
@@ -2516,16 +2780,16 @@
       <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="21">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="27">
         <f>E18+E13</f>
         <v>4250</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="28"/>
       <c r="H19" t="s">
         <v>85</v>
       </c>
@@ -2537,13 +2801,13 @@
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="H20" t="s">
         <v>82</v>
       </c>
@@ -2555,55 +2819,55 @@
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="21">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="27">
         <f>E19+E22</f>
         <v>4250</v>
       </c>
-      <c r="F23" s="24"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:13" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="24">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="28">
         <f>E23-E23*0%</f>
         <v>4250</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:13" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="G25" s="3"/>
@@ -2636,6 +2900,37 @@
     </row>
   </sheetData>
   <mergeCells count="47">
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B11:D11"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B18:D18"/>
     <mergeCell ref="A1:F1"/>
@@ -2652,37 +2947,6 @@
     <mergeCell ref="E11:F11"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2694,51 +2958,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="I14" sqref="A1:J14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="13" max="13" width="27.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="19"/>
       <c r="M2" t="s">
         <v>62</v>
       </c>
@@ -2747,26 +3011,26 @@
       </c>
     </row>
     <row r="3" spans="1:14" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14">
         <f>D4+D5+D6</f>
         <v>27000</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14">
         <f>I4+I5</f>
         <v>90000</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="15"/>
       <c r="M3" t="s">
         <v>68</v>
       </c>
@@ -2775,25 +3039,25 @@
       </c>
     </row>
     <row r="4" spans="1:14" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14">
         <f>(N3-N12)*N11</f>
         <v>5000</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14">
         <v>80000</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="M4" t="s">
         <v>69</v>
       </c>
@@ -2802,24 +3066,24 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="31.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14">
         <v>20000</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14">
         <v>10000</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="M5" t="s">
         <v>70</v>
       </c>
@@ -2828,20 +3092,20 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>100</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14">
         <v>2000</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="14"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="M6" t="s">
         <v>71</v>
       </c>
@@ -2850,26 +3114,26 @@
       </c>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14">
         <f>D8+D9</f>
         <v>56980</v>
       </c>
-      <c r="E7" s="15"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
         <f>I8+I9+I10</f>
         <v>42000</v>
       </c>
-      <c r="J7" s="15"/>
+      <c r="J7" s="14"/>
       <c r="L7" s="8"/>
       <c r="M7" t="s">
         <v>63</v>
@@ -2879,25 +3143,25 @@
       </c>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14">
         <f>N3*N5+N4*N6</f>
         <v>38500</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>6000</v>
       </c>
-      <c r="J8" s="14"/>
+      <c r="J8" s="15"/>
       <c r="M8" t="s">
         <v>67</v>
       </c>
@@ -2906,25 +3170,25 @@
       </c>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15">
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14">
         <f>N3*(N7*N9+Tableau379[[#This Row],[Colonne2]]*N10)*7</f>
         <v>18480</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14">
         <v>1000</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="14"/>
       <c r="M9" t="s">
         <v>72</v>
       </c>
@@ -2933,20 +3197,20 @@
       </c>
     </row>
     <row r="10" spans="1:14" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
+      <c r="A10" s="15"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14">
         <v>35000</v>
       </c>
-      <c r="J10" s="15"/>
+      <c r="J10" s="14"/>
       <c r="M10" t="s">
         <v>73</v>
       </c>
@@ -2955,26 +3219,26 @@
       </c>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14">
         <f>SUM(D12:E13)</f>
         <v>63020</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="15">
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="14">
         <f>I12</f>
         <v>15000</v>
       </c>
-      <c r="J11" s="14"/>
+      <c r="J11" s="15"/>
       <c r="M11" t="s">
         <v>77</v>
       </c>
@@ -2983,24 +3247,24 @@
       </c>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17">
         <v>7020</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19" t="s">
+      <c r="E12" s="17"/>
+      <c r="F12" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="18">
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="17">
         <v>15000</v>
       </c>
-      <c r="J12" s="19"/>
+      <c r="J12" s="16"/>
       <c r="M12" s="10" t="s">
         <v>99</v>
       </c>
@@ -3009,45 +3273,82 @@
       </c>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
         <v>56000</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
+      <c r="E13" s="17"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-      <c r="D14" s="18">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="17">
         <f>D11+D7+D3</f>
         <v>147000</v>
       </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="19" t="s">
+      <c r="E14" s="17"/>
+      <c r="F14" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="18">
+      <c r="G14" s="16"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="17">
         <f>I3+I7+I11</f>
         <v>147000</v>
       </c>
-      <c r="J14" s="18"/>
+      <c r="J14" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="53">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="A6:C6"/>
     <mergeCell ref="D6:E6"/>
     <mergeCell ref="F6:H6"/>
@@ -3064,43 +3365,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:J5"/>
   </mergeCells>
   <conditionalFormatting sqref="A7:J14 A1:J5">
     <cfRule type="colorScale" priority="9">
@@ -3150,84 +3414,84 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="8" max="8" width="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="26"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="25">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="26">
         <f>SUM(E5,E4)</f>
         <v>1403600</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="23"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="22">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="24">
         <f>I8*I10+I9*I11</f>
         <v>38500</v>
       </c>
-      <c r="F4" s="23"/>
+      <c r="F4" s="25"/>
       <c r="G4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="22">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="24">
         <f>((I8*I12*I14)+(I8*I13*I15))*365</f>
         <v>1365100</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="25"/>
       <c r="G5" t="s">
         <v>75</v>
       </c>
@@ -3236,28 +3500,28 @@
       <c r="A6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="21">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="27">
         <f>SUM(E7:F12)</f>
         <v>1401500</v>
       </c>
-      <c r="F6" s="24"/>
+      <c r="F6" s="28"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="21">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="27">
         <v>97500</v>
       </c>
-      <c r="F7" s="24"/>
+      <c r="F7" s="28"/>
       <c r="H7" t="s">
         <v>62</v>
       </c>
@@ -3268,16 +3532,16 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="21">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="27">
         <f>15000*12</f>
         <v>180000</v>
       </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="28"/>
       <c r="H8" t="s">
         <v>68</v>
       </c>
@@ -3290,15 +3554,15 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="21">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="27">
         <v>12000</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="27"/>
       <c r="H9" t="s">
         <v>69</v>
       </c>
@@ -3311,15 +3575,15 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="22">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="24">
         <v>6000</v>
       </c>
-      <c r="F10" s="23"/>
+      <c r="F10" s="25"/>
       <c r="H10" t="s">
         <v>70</v>
       </c>
@@ -3330,16 +3594,16 @@
     </row>
     <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="25">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="26">
         <f>(20000+15000*3+10000+6000*2+4000)*12</f>
         <v>1092000</v>
       </c>
-      <c r="F11" s="26"/>
+      <c r="F11" s="23"/>
       <c r="H11" t="s">
         <v>71</v>
       </c>
@@ -3350,15 +3614,15 @@
     </row>
     <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="25">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="26">
         <v>14000</v>
       </c>
-      <c r="F12" s="26"/>
+      <c r="F12" s="23"/>
       <c r="H12" t="s">
         <v>63</v>
       </c>
@@ -3371,16 +3635,16 @@
       <c r="A13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="21">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="27">
         <f>E3-E6</f>
         <v>2100</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="28"/>
       <c r="H13" t="s">
         <v>67</v>
       </c>
@@ -3393,16 +3657,16 @@
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="21">
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="27">
         <f>E15</f>
         <v>10000</v>
       </c>
-      <c r="F14" s="24"/>
+      <c r="F14" s="28"/>
       <c r="H14" t="s">
         <v>72</v>
       </c>
@@ -3413,15 +3677,15 @@
     </row>
     <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="22">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="24">
         <v>10000</v>
       </c>
-      <c r="F15" s="23"/>
+      <c r="F15" s="25"/>
       <c r="H15" t="s">
         <v>73</v>
       </c>
@@ -3434,16 +3698,16 @@
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="27">
         <f>E17</f>
         <v>2000</v>
       </c>
-      <c r="F16" s="24"/>
+      <c r="F16" s="28"/>
       <c r="H16" t="s">
         <v>79</v>
       </c>
@@ -3454,15 +3718,15 @@
     </row>
     <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="21">
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="27">
         <v>2000</v>
       </c>
-      <c r="F17" s="24"/>
+      <c r="F17" s="28"/>
       <c r="H17" t="s">
         <v>80</v>
       </c>
@@ -3475,16 +3739,16 @@
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="21">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="27">
         <f>E14-E16</f>
         <v>8000</v>
       </c>
-      <c r="F18" s="24"/>
+      <c r="F18" s="28"/>
       <c r="H18" t="s">
         <v>81</v>
       </c>
@@ -3497,16 +3761,16 @@
       <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="21">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="27">
         <f>E18+E13</f>
         <v>10100</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="28"/>
       <c r="H19" t="s">
         <v>85</v>
       </c>
@@ -3519,13 +3783,13 @@
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
       <c r="H20" t="s">
         <v>82</v>
       </c>
@@ -3538,96 +3802,59 @@
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="24"/>
-      <c r="F21" s="24"/>
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="28"/>
     </row>
     <row r="23" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="21">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="27">
         <f>E19+E22</f>
         <v>10100</v>
       </c>
-      <c r="F23" s="24"/>
+      <c r="F23" s="28"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="24">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="28">
         <f>E23-E23*0%</f>
         <v>10100</v>
       </c>
-      <c r="F24" s="24"/>
+      <c r="F24" s="28"/>
     </row>
     <row r="25" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="E23:F23"/>
     <mergeCell ref="B24:D24"/>
@@ -3638,6 +3865,43 @@
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3648,74 +3912,74 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
       <selection sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="14.42578125" customWidth="1"/>
     <col min="12" max="12" width="30.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:14" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="17"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="1:14" ht="37.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14">
         <f>D4+D5</f>
         <v>27500</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14">
         <f>I4+I5</f>
         <v>80000</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="15"/>
       <c r="L3" t="s">
         <v>62</v>
       </c>
@@ -3725,25 +3989,25 @@
       <c r="N3" s="10"/>
     </row>
     <row r="4" spans="1:14" ht="47.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14">
         <f>(Tableau37810512[[#This Row],[Colonne2]]-M17)*1000</f>
         <v>10000</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14">
         <v>80000</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
       <c r="L4" t="s">
         <v>68</v>
       </c>
@@ -3755,20 +4019,20 @@
       </c>
     </row>
     <row r="5" spans="1:14" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14">
         <v>17500</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15"/>
-      <c r="J5" s="14"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="15"/>
       <c r="L5" t="s">
         <v>69</v>
       </c>
@@ -3780,26 +4044,26 @@
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14">
         <f>D7+D8</f>
         <v>69450</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14">
         <f>I7+I8+I9</f>
         <v>42000</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="15"/>
       <c r="L6" t="s">
         <v>70</v>
       </c>
@@ -3809,25 +4073,25 @@
       <c r="N6" s="10"/>
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14">
         <f>M4*M6+M5*Tableau37810512[[#This Row],[Colonne2]]</f>
         <v>42150</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
         <v>6000</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="15"/>
       <c r="L7" t="s">
         <v>71</v>
       </c>
@@ -3837,25 +4101,25 @@
       <c r="N7" s="10"/>
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14">
         <f>M4*(Tableau37810512[[#This Row],[Colonne2]]*M10+M9*M11)*7</f>
         <v>27300</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>1000</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="14"/>
       <c r="L8" t="s">
         <v>63</v>
       </c>
@@ -3865,20 +4129,20 @@
       <c r="N8" s="10"/>
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14">
         <v>35000</v>
       </c>
-      <c r="J9" s="15"/>
+      <c r="J9" s="14"/>
       <c r="L9" t="s">
         <v>67</v>
       </c>
@@ -3888,26 +4152,26 @@
       <c r="N9" s="10"/>
     </row>
     <row r="10" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14">
         <f>SUM(D11:E12)</f>
         <v>40050</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="15">
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="14">
         <f>I11</f>
         <v>15000</v>
       </c>
-      <c r="J10" s="14"/>
+      <c r="J10" s="15"/>
       <c r="L10" t="s">
         <v>72</v>
       </c>
@@ -3917,24 +4181,24 @@
       <c r="N10" s="10"/>
     </row>
     <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="19"/>
-      <c r="C11" s="19"/>
-      <c r="D11" s="18">
+      <c r="B11" s="16"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17">
         <v>6050</v>
       </c>
-      <c r="E11" s="18"/>
-      <c r="F11" s="19" t="s">
+      <c r="E11" s="17"/>
+      <c r="F11" s="16" t="s">
         <v>98</v>
       </c>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="18">
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="17">
         <v>15000</v>
       </c>
-      <c r="J11" s="19"/>
+      <c r="J11" s="16"/>
       <c r="L11" t="s">
         <v>73</v>
       </c>
@@ -3944,20 +4208,20 @@
       <c r="N11" s="10"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="18">
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="17">
         <v>34000</v>
       </c>
-      <c r="E12" s="18"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16"/>
       <c r="L12" t="s">
         <v>79</v>
       </c>
@@ -3967,26 +4231,26 @@
       <c r="N12" s="10"/>
     </row>
     <row r="13" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="19"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="17">
         <f>D10+D6+D3</f>
         <v>137000</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="18">
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="17">
         <f>I3+I6+I10</f>
         <v>137000</v>
       </c>
-      <c r="J13" s="18"/>
+      <c r="J13" s="17"/>
       <c r="L13" t="s">
         <v>80</v>
       </c>
@@ -4033,46 +4297,6 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="I13:J13"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:H12"/>
-    <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A11:C11"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="F11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:J5"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:H3"/>
@@ -4082,6 +4306,46 @@
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="A11:C11"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="F11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:H12"/>
+    <mergeCell ref="I12:J12"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:J13">
     <cfRule type="colorScale" priority="1">
@@ -4101,84 +4365,84 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection sqref="A1:F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="8" max="8" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="30"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="31">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="32">
         <f>SUM(E5,E4)</f>
         <v>1465650</v>
       </c>
-      <c r="F3" s="31"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="32">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="31">
         <f>I8*I10+I9*I11</f>
         <v>42150</v>
       </c>
-      <c r="F4" s="32"/>
+      <c r="F4" s="31"/>
       <c r="G4" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="32">
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="31">
         <f>((I8*I12*I14)+(I8*I13*I15))*365</f>
         <v>1423500</v>
       </c>
-      <c r="F5" s="32"/>
+      <c r="F5" s="31"/>
       <c r="G5" t="s">
         <v>75</v>
       </c>
@@ -4187,29 +4451,29 @@
       <c r="A6" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="33">
+      <c r="C6" s="22"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="30">
         <f>SUM(E7:F12)</f>
         <v>1400500</v>
       </c>
-      <c r="F6" s="33"/>
+      <c r="F6" s="30"/>
     </row>
     <row r="7" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="33">
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="30">
         <f>1000*60+20500</f>
         <v>80500</v>
       </c>
-      <c r="F7" s="33"/>
+      <c r="F7" s="30"/>
       <c r="H7" t="s">
         <v>62</v>
       </c>
@@ -4220,16 +4484,16 @@
     </row>
     <row r="8" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="33">
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="30">
         <f>15000*12</f>
         <v>180000</v>
       </c>
-      <c r="F8" s="33"/>
+      <c r="F8" s="30"/>
       <c r="H8" t="s">
         <v>68</v>
       </c>
@@ -4242,16 +4506,16 @@
     </row>
     <row r="9" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="33">
+      <c r="C9" s="22"/>
+      <c r="D9" s="22"/>
+      <c r="E9" s="30">
         <f>1000*12</f>
         <v>12000</v>
       </c>
-      <c r="F9" s="33"/>
+      <c r="F9" s="30"/>
       <c r="H9" t="s">
         <v>69</v>
       </c>
@@ -4264,15 +4528,15 @@
     </row>
     <row r="10" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="32">
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="31">
         <v>6000</v>
       </c>
-      <c r="F10" s="32"/>
+      <c r="F10" s="31"/>
       <c r="H10" t="s">
         <v>70</v>
       </c>
@@ -4283,16 +4547,16 @@
     </row>
     <row r="11" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="31">
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="32">
         <f>(15000*3+20000+10000+6000*2+4000)*12</f>
         <v>1092000</v>
       </c>
-      <c r="F11" s="31"/>
+      <c r="F11" s="32"/>
       <c r="H11" t="s">
         <v>71</v>
       </c>
@@ -4303,15 +4567,15 @@
     </row>
     <row r="12" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="31">
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="32">
         <v>30000</v>
       </c>
-      <c r="F12" s="31"/>
+      <c r="F12" s="32"/>
       <c r="H12" t="s">
         <v>63</v>
       </c>
@@ -4324,16 +4588,16 @@
       <c r="A13" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="33">
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="30">
         <f>E3-E6</f>
         <v>65150</v>
       </c>
-      <c r="F13" s="33"/>
+      <c r="F13" s="30"/>
       <c r="H13" t="s">
         <v>67</v>
       </c>
@@ -4346,16 +4610,16 @@
       <c r="A14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="33">
+      <c r="C14" s="29"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="30">
         <f>E15</f>
         <v>7000</v>
       </c>
-      <c r="F14" s="33"/>
+      <c r="F14" s="30"/>
       <c r="H14" t="s">
         <v>72</v>
       </c>
@@ -4366,15 +4630,15 @@
     </row>
     <row r="15" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6"/>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="32">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="31">
         <v>7000</v>
       </c>
-      <c r="F15" s="32"/>
+      <c r="F15" s="31"/>
       <c r="H15" t="s">
         <v>73</v>
       </c>
@@ -4387,16 +4651,16 @@
       <c r="A16" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="33">
+      <c r="C16" s="22"/>
+      <c r="D16" s="22"/>
+      <c r="E16" s="30">
         <f>E17</f>
         <v>0</v>
       </c>
-      <c r="F16" s="33"/>
+      <c r="F16" s="30"/>
       <c r="H16" t="s">
         <v>79</v>
       </c>
@@ -4407,11 +4671,11 @@
     </row>
     <row r="17" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="33"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
       <c r="H17" t="s">
         <v>80</v>
       </c>
@@ -4424,16 +4688,16 @@
       <c r="A18" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="28"/>
-      <c r="D18" s="28"/>
-      <c r="E18" s="33">
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="30">
         <f>E14-E16</f>
         <v>7000</v>
       </c>
-      <c r="F18" s="33"/>
+      <c r="F18" s="30"/>
       <c r="H18" t="s">
         <v>81</v>
       </c>
@@ -4446,16 +4710,16 @@
       <c r="A19" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="33">
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="30">
         <f>E18+E13</f>
         <v>72150</v>
       </c>
-      <c r="F19" s="33"/>
+      <c r="F19" s="30"/>
       <c r="H19" t="s">
         <v>85</v>
       </c>
@@ -4468,13 +4732,13 @@
       <c r="A20" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
+      <c r="C20" s="22"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
       <c r="H20" t="s">
         <v>82</v>
       </c>
@@ -4487,29 +4751,29 @@
       <c r="A21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="20" t="s">
+      <c r="B21" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="28">
+      <c r="C21" s="22"/>
+      <c r="D21" s="22"/>
+      <c r="E21" s="20">
         <f>E22</f>
         <v>5925</v>
       </c>
-      <c r="F21" s="28"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="28">
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="20">
         <f>(10*3+7*5)*3*15+3*1000</f>
         <v>5925</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="20"/>
       <c r="G22" t="s">
         <v>97</v>
       </c>
@@ -4518,50 +4782,83 @@
       <c r="A23" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C23" s="28"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28">
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20">
         <f>-E22</f>
         <v>-5925</v>
       </c>
-      <c r="F23" s="28"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="28" t="s">
+      <c r="B24" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="28"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="33">
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="30">
         <f>E19+E23</f>
         <v>66225</v>
       </c>
-      <c r="F24" s="33"/>
+      <c r="F24" s="30"/>
     </row>
     <row r="25" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="C25" s="28"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="24">
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="28">
         <f>E24-E24*0%</f>
         <v>66225</v>
       </c>
-      <c r="F25" s="24"/>
+      <c r="F25" s="28"/>
     </row>
     <row r="26" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="E24:F24"/>
@@ -4576,41 +4873,8 @@
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="E14:F14"/>
     <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="E23:F23"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:F4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4621,263 +4885,300 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:10" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:10" ht="33" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14" t="s">
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14" t="s">
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="14"/>
+      <c r="J2" s="15"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="15">
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="14">
         <v>27500</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14" t="s">
+      <c r="E3" s="15"/>
+      <c r="F3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15">
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="14">
         <f>I4+I5</f>
         <v>90000</v>
       </c>
-      <c r="J3" s="14"/>
+      <c r="J3" s="15"/>
     </row>
     <row r="4" spans="1:10" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="15">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="14">
         <v>20000</v>
       </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="14">
         <v>80000</v>
       </c>
-      <c r="J4" s="14"/>
+      <c r="J4" s="15"/>
     </row>
     <row r="5" spans="1:10" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="15">
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="14">
         <v>7500</v>
       </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="15">
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="14">
         <v>10000</v>
       </c>
-      <c r="J5" s="14"/>
+      <c r="J5" s="15"/>
     </row>
     <row r="6" spans="1:10" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="15">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="14">
         <f>SUM(D7:E8)</f>
         <v>85500</v>
       </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="15">
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="14">
         <f>SUM(I7:J9)</f>
         <v>52100</v>
       </c>
-      <c r="J6" s="14"/>
+      <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="15">
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="14">
         <v>55000</v>
       </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="15">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="14">
         <v>500</v>
       </c>
-      <c r="J7" s="14"/>
+      <c r="J7" s="15"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="15">
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="14">
         <v>30500</v>
       </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
+      <c r="E8" s="15"/>
+      <c r="F8" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="15">
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="14">
         <v>20000</v>
       </c>
-      <c r="J8" s="15"/>
+      <c r="J8" s="14"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14" t="s">
+      <c r="A9" s="15"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="15">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="14">
         <v>31600</v>
       </c>
-      <c r="J9" s="14"/>
+      <c r="J9" s="15"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="15">
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="14">
         <f>SUM(D11:E12)</f>
         <v>29100</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
     </row>
     <row r="11" spans="1:10" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="15">
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="14">
         <v>5100</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
     </row>
     <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+      <c r="A12" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="15">
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="14">
         <v>24000</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="15">
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="14">
         <f>D10+D6+D3</f>
         <v>142100</v>
       </c>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14" t="s">
+      <c r="E13" s="15"/>
+      <c r="F13" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="15">
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="14">
         <f>I6+I3</f>
         <v>142100</v>
       </c>
-      <c r="J13" s="14"/>
+      <c r="J13" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="I8:J8"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:H7"/>
+    <mergeCell ref="I7:J7"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:H9"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:H10"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="A13:C13"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:H13"/>
@@ -4890,43 +5191,6 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="I12:J12"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:H9"/>
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="F10:H10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:H8"/>
-    <mergeCell ref="I8:J8"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:H7"/>
-    <mergeCell ref="I7:J7"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:H5"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="I2:J2"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:J13">
     <cfRule type="colorScale" priority="3">
@@ -4944,14 +5208,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection sqref="A1:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
     <col min="2" max="4" width="11.5703125" customWidth="1"/>

</xml_diff>